<commit_message>
good result gif plot
</commit_message>
<xml_diff>
--- a/results/hpe_action_experiments.xlsx
+++ b/results/hpe_action_experiments.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9405" windowHeight="9990" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FiLM" sheetId="1" r:id="rId1"/>
     <sheet name="Extra" sheetId="3" r:id="rId2"/>
     <sheet name="Overall" sheetId="2" r:id="rId3"/>
-    <sheet name="OverallTrainPlots" sheetId="4" r:id="rId4"/>
-    <sheet name="OverallValPlots" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="OverallTrainPlots" sheetId="4" r:id="rId5"/>
+    <sheet name="OverallValPlots" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Experiment</t>
   </si>
@@ -135,6 +137,15 @@
   <si>
     <t>0514_1801</t>
   </si>
+  <si>
+    <t>CombinedTrivialBaseline</t>
+  </si>
+  <si>
+    <t>AVG3DERROR_MM</t>
+  </si>
+  <si>
+    <t>ACC_%</t>
+  </si>
 </sst>
 </file>
 
@@ -225,6 +236,416 @@
   <c:chart>
     <c:title>
       <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG3DERROR_MM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="35"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>11.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.340000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>26.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-173C-4C30-B5FB-B4F22CF750BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1281222416"/>
+        <c:axId val="1281229488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1281222416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1281229488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1281229488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1281222416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1553,7 +1974,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1628,7 +2048,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1695,7 +2114,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1735,7 +2154,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3066,7 +3484,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3141,7 +3558,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3288,8 +3704,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3316,8 +3772,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3397,11 +3853,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3412,11 +3863,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3428,7 +3874,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3448,9 +3894,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3463,10 +3906,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3506,22 +3949,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -3626,8 +4070,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3759,19 +4203,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3785,6 +4230,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4320,7 +4776,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>490538</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4355,7 +5362,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4842,9 +5849,95 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>11.48</v>
+      </c>
+      <c r="C6">
+        <v>26.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>23.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>26.6</v>
+      </c>
+      <c r="C8">
+        <v>23.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>22.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>40.340000000000003</v>
+      </c>
+      <c r="C10">
+        <v>21.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>42.34</v>
+      </c>
+      <c r="C11">
+        <v>20.010000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>83</v>
+      </c>
+      <c r="C12">
+        <v>10.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -5482,7 +6575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>

</xml_diff>